<commit_message>
Updated maximum loan amount worksheet with desired loan amount and stats
</commit_message>
<xml_diff>
--- a/assets/worksheets/Maximum-Loan-Amount.xlsx
+++ b/assets/worksheets/Maximum-Loan-Amount.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Property Parameters</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Indicated Direct Cap. Value</t>
+  </si>
+  <si>
+    <t>Indicated Gross Rent Multiplier</t>
   </si>
   <si>
     <t>Lender Parameters</t>
@@ -102,18 +105,34 @@
   <si>
     <t>Maximum Loan (rounded)</t>
   </si>
+  <si>
+    <t>Desired Loan Amount</t>
+  </si>
+  <si>
+    <t>LTV</t>
+  </si>
+  <si>
+    <t>Monthly Debt Service</t>
+  </si>
+  <si>
+    <t>Monthly Net Cash Flow</t>
+  </si>
+  <si>
+    <t>Debt Service Coverage Ratio (DSCR)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0 &quot;years&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.00&quot;x&quot;"/>
+    <numFmt numFmtId="170" formatCode="0 &quot;years&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -180,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -214,6 +233,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -238,7 +260,7 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="170" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -261,6 +283,12 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="169" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,8 +718,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="12">
+        <f>C12/C5</f>
+        <v>12.33333333</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -720,7 +753,7 @@
     <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="12"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -749,9 +782,9 @@
     <row r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -779,8 +812,8 @@
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="14" t="s">
-        <v>13</v>
+      <c r="B16" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="9">
         <v>0.7</v>
@@ -811,11 +844,11 @@
       <c r="AA16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="15" t="s">
-        <v>14</v>
+      <c r="A17" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7">
         <f>C12*C16</f>
@@ -849,7 +882,7 @@
     <row r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -877,10 +910,10 @@
     </row>
     <row r="19">
       <c r="A19" s="4"/>
-      <c r="B19" s="14" t="s">
-        <v>16</v>
+      <c r="B19" s="15" t="s">
+        <v>17</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="18">
         <v>1.2</v>
       </c>
       <c r="D19" s="4"/>
@@ -911,9 +944,9 @@
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="19">
         <v>0.0475</v>
       </c>
       <c r="D20" s="4"/>
@@ -944,9 +977,9 @@
     <row r="21">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="20">
         <v>30.0</v>
       </c>
       <c r="D21" s="4"/>
@@ -977,9 +1010,9 @@
     <row r="22">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="21">
         <f>pmt(C20/12,C21*12,-1)*12</f>
         <v>0.06259768038</v>
       </c>
@@ -1011,9 +1044,9 @@
     <row r="23">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="22">
         <f>C22*C19</f>
         <v>0.07511721646</v>
       </c>
@@ -1043,11 +1076,11 @@
       <c r="AA23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
-        <v>21</v>
+      <c r="A24" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" s="7">
         <f>C10/C23</f>
@@ -1108,11 +1141,11 @@
       <c r="AA25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="15"/>
-      <c r="B26" s="22" t="s">
-        <v>23</v>
+      <c r="A26" s="16"/>
+      <c r="B26" s="23" t="s">
+        <v>24</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="24">
         <f>min(C17,C24)</f>
         <v>1479687.417</v>
       </c>
@@ -1142,11 +1175,11 @@
       <c r="AA26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25" t="s">
-        <v>24</v>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26" t="s">
+        <v>25</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="27">
         <f>ROUNDDOWN(C26,-3)</f>
         <v>1479000</v>
       </c>
@@ -1177,8 +1210,13 @@
     </row>
     <row r="28">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="28">
+        <f>C27</f>
+        <v>1479000</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1206,8 +1244,13 @@
     </row>
     <row r="29">
       <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="14">
+        <f>C28/C12</f>
+        <v>0.6662162162</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -1235,8 +1278,13 @@
     </row>
     <row r="30">
       <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="3">
+        <f>C28*C22/12</f>
+        <v>7715.164107</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1264,8 +1312,13 @@
     </row>
     <row r="31">
       <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="3">
+        <f>C10/12-C30</f>
+        <v>1547.335893</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1293,8 +1346,13 @@
     </row>
     <row r="32">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="29">
+        <f>C10/12/C30</f>
+        <v>1.200557742</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -29682,6 +29740,35 @@
       <c r="Z1010" s="4"/>
       <c r="AA1010" s="4"/>
     </row>
+    <row r="1011">
+      <c r="A1011" s="4"/>
+      <c r="B1011" s="4"/>
+      <c r="C1011" s="4"/>
+      <c r="D1011" s="4"/>
+      <c r="E1011" s="4"/>
+      <c r="F1011" s="4"/>
+      <c r="G1011" s="4"/>
+      <c r="H1011" s="4"/>
+      <c r="I1011" s="4"/>
+      <c r="J1011" s="4"/>
+      <c r="K1011" s="4"/>
+      <c r="L1011" s="4"/>
+      <c r="M1011" s="4"/>
+      <c r="N1011" s="4"/>
+      <c r="O1011" s="4"/>
+      <c r="P1011" s="4"/>
+      <c r="Q1011" s="4"/>
+      <c r="R1011" s="4"/>
+      <c r="S1011" s="4"/>
+      <c r="T1011" s="4"/>
+      <c r="U1011" s="4"/>
+      <c r="V1011" s="4"/>
+      <c r="W1011" s="4"/>
+      <c r="X1011" s="4"/>
+      <c r="Y1011" s="4"/>
+      <c r="Z1011" s="4"/>
+      <c r="AA1011" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>